<commit_message>
Main only runs algos once now
</commit_message>
<xml_diff>
--- a/LAB02/StatsLab2.xlsx
+++ b/LAB02/StatsLab2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydendonofrio/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haydendonofrio/CLionProjects/CSE3353/LAB02/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A30C45-8AD4-C344-87C8-4834959FA5A2}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE736D51-1367-8A43-AE8E-D68AC072918D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14260" xr2:uid="{3506A316-8761-A240-B085-8C7A409D7608}"/>
   </bookViews>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9D71696-676E-9641-9BA5-007AB501BB5D}">
   <dimension ref="A1:AD32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N10" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23:W23"/>
+    <sheetView tabSelected="1" topLeftCell="N9" workbookViewId="0">
+      <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1919,10 +1919,10 @@
         <v>340</v>
       </c>
       <c r="M23">
-        <v>248</v>
+        <v>348</v>
       </c>
       <c r="N23">
-        <v>227</v>
+        <v>327</v>
       </c>
       <c r="Q23" t="s">
         <v>9</v>
@@ -2416,22 +2416,22 @@
         <v>9</v>
       </c>
       <c r="B31">
-        <v>520</v>
+        <v>535</v>
       </c>
       <c r="C31">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="D31">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="E31">
-        <v>319</v>
+        <v>414</v>
       </c>
       <c r="F31">
-        <v>247</v>
+        <v>333</v>
       </c>
       <c r="G31">
-        <v>233</v>
+        <v>345</v>
       </c>
       <c r="H31" t="s">
         <v>9</v>
@@ -2449,10 +2449,10 @@
         <v>323</v>
       </c>
       <c r="M31">
-        <v>251</v>
+        <v>351</v>
       </c>
       <c r="N31">
-        <v>254</v>
+        <v>354</v>
       </c>
       <c r="Q31" t="s">
         <v>9</v>

</xml_diff>